<commit_message>
Uploaded new log riskprem
</commit_message>
<xml_diff>
--- a/datasets/M1_riskprem_exante_log.xlsx
+++ b/datasets/M1_riskprem_exante_log.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -654,659 +654,609 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>41365</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>-inf</t>
-        </is>
+        <v>41518</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.02691559138294862</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>41395</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>-inf</t>
-        </is>
+        <v>41548</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.03768226149323169</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>41426</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>-inf</t>
-        </is>
+        <v>41579</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.009328253105357431</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>41456</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>-inf</t>
-        </is>
+        <v>41609</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-0.007326696754221629</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>41487</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>-inf</t>
-        </is>
+        <v>41640</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.02879757008862111</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>41518</v>
+        <v>41671</v>
       </c>
       <c r="B33" t="n">
-        <v>0.02691559138294862</v>
+        <v>-0.00436000259131012</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>41548</v>
+        <v>41699</v>
       </c>
       <c r="B34" t="n">
-        <v>0.03768226149323169</v>
+        <v>-0.0196189713351441</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>41579</v>
+        <v>41730</v>
       </c>
       <c r="B35" t="n">
-        <v>0.009328253105357431</v>
+        <v>-0.01720302331342762</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>41609</v>
+        <v>41760</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.007326696754221629</v>
+        <v>-0.01740472376737029</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>41640</v>
+        <v>41791</v>
       </c>
       <c r="B37" t="n">
-        <v>0.02879757008862111</v>
+        <v>-0.01050632708778454</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>41671</v>
+        <v>41821</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.00436000259131012</v>
+        <v>-0.0009015971614543541</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>41699</v>
+        <v>41852</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.0196189713351441</v>
+        <v>-0.02186730698961913</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>41730</v>
+        <v>41883</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.01720302331342762</v>
+        <v>-0.007720196679194863</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>41760</v>
+        <v>41913</v>
       </c>
       <c r="B41" t="n">
-        <v>-0.01740472376737029</v>
+        <v>0.02329525003096519</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>41791</v>
+        <v>41944</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.01050632708778454</v>
+        <v>0.02617674133688973</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>41821</v>
+        <v>41974</v>
       </c>
       <c r="B43" t="n">
-        <v>-0.0009015971614543541</v>
+        <v>0.005211536642448028</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>41852</v>
+        <v>42005</v>
       </c>
       <c r="B44" t="n">
-        <v>-0.02186730698961913</v>
+        <v>0.02273875715326237</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>41883</v>
+        <v>42036</v>
       </c>
       <c r="B45" t="n">
-        <v>-0.007720196679194863</v>
+        <v>-0.01999149222445708</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>41913</v>
+        <v>42064</v>
       </c>
       <c r="B46" t="n">
-        <v>0.02329525003096519</v>
+        <v>0.1201934258998716</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>41944</v>
+        <v>42095</v>
       </c>
       <c r="B47" t="n">
-        <v>0.02617674133688973</v>
+        <v>-0.006795740229209086</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>41974</v>
+        <v>42125</v>
       </c>
       <c r="B48" t="n">
-        <v>0.005211536642448028</v>
+        <v>-0.02685762357626824</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>42005</v>
+        <v>42156</v>
       </c>
       <c r="B49" t="n">
-        <v>0.02273875715326237</v>
+        <v>0.02582130127211581</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>42036</v>
+        <v>42186</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.01999149222445708</v>
+        <v>0.03552702775153913</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>42064</v>
+        <v>42217</v>
       </c>
       <c r="B51" t="n">
-        <v>0.1201934258998716</v>
+        <v>0.04290740498071908</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>42095</v>
+        <v>42248</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.006795740229209086</v>
+        <v>0.0131774698632198</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>42125</v>
+        <v>42278</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.02685762357626824</v>
+        <v>0.02978382742925741</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>42156</v>
+        <v>42309</v>
       </c>
       <c r="B54" t="n">
-        <v>0.02582130127211581</v>
+        <v>0.03318113779655417</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>42186</v>
+        <v>42339</v>
       </c>
       <c r="B55" t="n">
-        <v>0.03552702775153913</v>
+        <v>-0.002918632822138695</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>42217</v>
+        <v>42370</v>
       </c>
       <c r="B56" t="n">
-        <v>0.04290740498071908</v>
+        <v>-0.01121665049203827</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>42248</v>
+        <v>42401</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0131774698632198</v>
+        <v>-0.008308803152131358</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>42278</v>
+        <v>42430</v>
       </c>
       <c r="B58" t="n">
-        <v>0.02978382742925741</v>
+        <v>-0.02491492558017515</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>42309</v>
+        <v>42461</v>
       </c>
       <c r="B59" t="n">
-        <v>0.03318113779655417</v>
+        <v>0.04091265447548714</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>42339</v>
+        <v>42491</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.002918632822138695</v>
+        <v>0.005693608006967915</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>42370</v>
+        <v>42522</v>
       </c>
       <c r="B61" t="n">
-        <v>-0.01121665049203827</v>
+        <v>-0.007026300319253631</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>42401</v>
+        <v>42552</v>
       </c>
       <c r="B62" t="n">
-        <v>-0.008308803152131358</v>
+        <v>0.03636107786259569</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>42430</v>
+        <v>42583</v>
       </c>
       <c r="B63" t="n">
-        <v>-0.02491492558017515</v>
+        <v>0.01279271211429842</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>42461</v>
+        <v>42614</v>
       </c>
       <c r="B64" t="n">
-        <v>0.04091265447548714</v>
+        <v>-0.004761205134110776</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>42491</v>
+        <v>42644</v>
       </c>
       <c r="B65" t="n">
-        <v>0.005693608006967915</v>
+        <v>-0.0170417419885327</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>42522</v>
+        <v>42675</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.007026300319253631</v>
+        <v>0.06646596505282398</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>42552</v>
+        <v>42705</v>
       </c>
       <c r="B67" t="n">
-        <v>0.03636107786259569</v>
+        <v>0.03460343244476255</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>42583</v>
+        <v>42736</v>
       </c>
       <c r="B68" t="n">
-        <v>0.01279271211429842</v>
+        <v>-0.007831765706510733</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>42614</v>
+        <v>42767</v>
       </c>
       <c r="B69" t="n">
-        <v>-0.004761205134110776</v>
+        <v>0.02504518787138696</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>42644</v>
+        <v>42795</v>
       </c>
       <c r="B70" t="n">
-        <v>-0.0170417419885327</v>
+        <v>-0.04079542646381094</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>42675</v>
+        <v>42826</v>
       </c>
       <c r="B71" t="n">
-        <v>0.06646596505282398</v>
+        <v>-0.09974508182049296</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>42705</v>
+        <v>42856</v>
       </c>
       <c r="B72" t="n">
-        <v>0.03460343244476255</v>
+        <v>-0.002808990967995344</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>42736</v>
+        <v>42887</v>
       </c>
       <c r="B73" t="n">
-        <v>-0.007831765706510733</v>
+        <v>-0.01054518587030063</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>42767</v>
+        <v>42917</v>
       </c>
       <c r="B74" t="n">
-        <v>0.02504518787138696</v>
+        <v>0.01026485850582108</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>42795</v>
+        <v>42948</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.04079542646381094</v>
+        <v>-0.005002333805427839</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>42826</v>
+        <v>42979</v>
       </c>
       <c r="B76" t="n">
-        <v>-0.09974508182049296</v>
+        <v>-0.01527572448170082</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>42856</v>
+        <v>43009</v>
       </c>
       <c r="B77" t="n">
-        <v>-0.002808990967995344</v>
+        <v>0.007288802893256008</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>42887</v>
+        <v>43040</v>
       </c>
       <c r="B78" t="n">
-        <v>-0.01054518587030063</v>
+        <v>0.03262560141975288</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>42917</v>
+        <v>43070</v>
       </c>
       <c r="B79" t="n">
-        <v>0.01026485850582108</v>
+        <v>0.02012033134243013</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>42948</v>
+        <v>43101</v>
       </c>
       <c r="B80" t="n">
-        <v>-0.005002333805427839</v>
+        <v>0.01820261284721708</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>42979</v>
+        <v>43132</v>
       </c>
       <c r="B81" t="n">
-        <v>-0.01527572448170082</v>
+        <v>0.008267552122181302</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>43009</v>
+        <v>43160</v>
       </c>
       <c r="B82" t="n">
-        <v>0.007288802893256008</v>
+        <v>0.03706707089569439</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>43040</v>
+        <v>43191</v>
       </c>
       <c r="B83" t="n">
-        <v>0.03262560141975288</v>
+        <v>0.001943211682393118</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>43070</v>
+        <v>43221</v>
       </c>
       <c r="B84" t="n">
-        <v>0.02012033134243013</v>
+        <v>-0.03768654906313377</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>43101</v>
+        <v>43252</v>
       </c>
       <c r="B85" t="n">
-        <v>0.01820261284721708</v>
+        <v>0.02685029638437141</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>43132</v>
+        <v>43282</v>
       </c>
       <c r="B86" t="n">
-        <v>0.008267552122181302</v>
+        <v>0.04915239342893075</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>43160</v>
+        <v>43313</v>
       </c>
       <c r="B87" t="n">
-        <v>0.03706707089569439</v>
+        <v>0.02861558673260393</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>43191</v>
+        <v>43344</v>
       </c>
       <c r="B88" t="n">
-        <v>0.001943211682393118</v>
+        <v>0.03990013275718382</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>43221</v>
+        <v>43374</v>
       </c>
       <c r="B89" t="n">
-        <v>-0.03768654906313377</v>
+        <v>0.04934036201137547</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>43252</v>
+        <v>43405</v>
       </c>
       <c r="B90" t="n">
-        <v>0.02685029638437141</v>
+        <v>0.02021182437032918</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>43282</v>
+        <v>43435</v>
       </c>
       <c r="B91" t="n">
-        <v>0.04915239342893075</v>
+        <v>0.04644364826554182</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>43313</v>
+        <v>43466</v>
       </c>
       <c r="B92" t="n">
-        <v>0.02861558673260393</v>
+        <v>0.08010129768779141</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>43344</v>
+        <v>43497</v>
       </c>
       <c r="B93" t="n">
-        <v>0.03990013275718382</v>
+        <v>0.06646672376997682</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>43374</v>
+        <v>43525</v>
       </c>
       <c r="B94" t="n">
-        <v>0.04934036201137547</v>
+        <v>-0.004669921615419993</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>43405</v>
+        <v>43556</v>
       </c>
       <c r="B95" t="n">
-        <v>0.02021182437032918</v>
+        <v>-0.01408462961026869</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>43435</v>
+        <v>43586</v>
       </c>
       <c r="B96" t="n">
-        <v>0.04644364826554182</v>
+        <v>0.08569952031999048</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>43466</v>
+        <v>43617</v>
       </c>
       <c r="B97" t="n">
-        <v>0.08010129768779141</v>
+        <v>0.04809490706333411</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>43497</v>
+        <v>43647</v>
       </c>
       <c r="B98" t="n">
-        <v>0.06646672376997682</v>
+        <v>0.0254521291465795</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>43525</v>
+        <v>43678</v>
       </c>
       <c r="B99" t="n">
-        <v>-0.004669921615419993</v>
+        <v>0.1238628635133538</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>43556</v>
+        <v>43709</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.01408462961026869</v>
+        <v>0.05462232302107554</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>43586</v>
+        <v>43739</v>
       </c>
       <c r="B101" t="n">
-        <v>0.08569952031999048</v>
+        <v>0.05665187125436073</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>43617</v>
+        <v>43770</v>
       </c>
       <c r="B102" t="n">
-        <v>0.04809490706333411</v>
+        <v>0.0736553126730226</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>43647</v>
+        <v>43800</v>
       </c>
       <c r="B103" t="n">
-        <v>0.0254521291465795</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="2" t="n">
-        <v>43678</v>
-      </c>
-      <c r="B104" t="n">
-        <v>0.1238628635133538</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="2" t="n">
-        <v>43709</v>
-      </c>
-      <c r="B105" t="n">
-        <v>0.05462232302107554</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="2" t="n">
-        <v>43739</v>
-      </c>
-      <c r="B106" t="n">
-        <v>0.05665187125436073</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="2" t="n">
-        <v>43770</v>
-      </c>
-      <c r="B107" t="n">
-        <v>0.0736553126730226</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="2" t="n">
-        <v>43800</v>
-      </c>
-      <c r="B108" t="n">
         <v>0.02823909613485797</v>
       </c>
     </row>

</xml_diff>